<commit_message>
working on getting month
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory8\OneDrive\Documents\UiPath\GenerateYearlyReportProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD85CF54-1A0C-40E4-8A5C-2C59F1C52486}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F3A6C6A-FC07-4754-897F-8DD77C032970}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,10 +125,10 @@
     <t>https://acme-test.uipath.com/account/login</t>
   </si>
   <si>
-    <t>C:\Users\Cory8\OneDrive\Documents\UiPath\GenerateYearlyReportProcess\Temp</t>
+    <t>ReportsDownloadPath</t>
   </si>
   <si>
-    <t>ReportsDownloadPath</t>
+    <t>C:\Users\Cory8\OneDrive\Documents\UiPath\GenerateYearlyReportProcess\Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -587,10 +587,10 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>